<commit_message>
correciones de hoja de calculo de rutas de api
</commit_message>
<xml_diff>
--- a/Rutas_proyecto.xlsx
+++ b/Rutas_proyecto.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t xml:space="preserve">rutas  request</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cesar león </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeferson  Redondo</t>
   </si>
   <si>
     <t xml:space="preserve">CASOS DE USUARIO</t>
@@ -239,7 +242,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,7 +264,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF81ACA6"/>
-        <bgColor rgb="FF9999FF"/>
+        <bgColor rgb="FF729FCF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF81ACA6"/>
       </patternFill>
     </fill>
     <fill>
@@ -340,7 +349,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -369,7 +378,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -381,11 +390,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -432,7 +449,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFA9D18E"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFD7"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -654,10 +671,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -885,18 +902,23 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="10" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -927,83 +949,83 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="117.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="68.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="117.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="68.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>48</v>
       </c>
+      <c r="B1" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>49</v>
+      <c r="B2" s="14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>50</v>
+      <c r="B3" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>51</v>
+      <c r="B4" s="14" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>52</v>
+      <c r="B5" s="15" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>54</v>
       </c>
+      <c r="B6" s="15" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="16" t="s">
         <v>56</v>
       </c>
+      <c r="B7" s="16" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>